<commit_message>
emissions graph now uses technolgy col
</commit_message>
<xml_diff>
--- a/config/plotting_config_and_timeslices.xlsx
+++ b/config/plotting_config_and_timeslices.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\power-model\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1000DC78-1EA1-49A4-9FB8-2A3930DED42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A309E3BF-36A0-432D-B12F-87EB4E8EC873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FUEL" sheetId="1" r:id="rId1"/>
+    <sheet name="INPUT_FUEL" sheetId="1" r:id="rId1"/>
     <sheet name="POWERPLANT" sheetId="5" r:id="rId2"/>
     <sheet name="plotting_name_to_color" sheetId="2" r:id="rId3"/>
     <sheet name="timeslices" sheetId="4" r:id="rId4"/>
@@ -426,6 +426,161 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82785BF2-0CB8-F2B2-5B9A-09AB9117A434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6562725" y="1381125"/>
+          <a:ext cx="5543550" cy="2466975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Not the same as the FUEL variable in Osemosys input</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DE96D83-A72A-4029-910B-1F8A37A3A5CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5753100" y="1628775"/>
+          <a:ext cx="5543550" cy="2463800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Not used currently because emissions time series uses INPUT_FUEL</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> sheet</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -694,7 +849,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -824,6 +979,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -831,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC71A03-AE6D-4049-B24E-310B3F034CAE}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1042,7 +1198,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873EB18-23BE-4A8F-8810-A9B73B0B6195}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1700,5 +1856,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>